<commit_message>
rm location resource (#281) 5c71137e5f8f61ba9b560abbb0ffa30162a843b1
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-as-dp-device.xlsx
+++ b/main/ig/StructureDefinition-as-dp-device.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-08T12:28:03+00:00</t>
+    <t>2025-10-08T12:56:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -14641,7 +14641,7 @@
         <v>78</v>
       </c>
       <c r="G111" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H111" t="s" s="2">
         <v>77</v>

</xml_diff>

<commit_message>
Déplacement des tags MS (Must Support) (#282)
* refact MS device

* MV MS to dp & dr profiles

* add ruleset 64379fb98cae727ba29a570433c6196bc7c5737a
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-as-dp-device.xlsx
+++ b/main/ig/StructureDefinition-as-dp-device.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-08T13:03:27+00:00</t>
+    <t>2025-10-10T07:08:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1311,7 +1311,7 @@
     <t>Device.status</t>
   </si>
   <si>
-    <t>Le matériel est-il actif? active | inactive</t>
+    <t>Le matériel est-il actif ? active | inactive</t>
   </si>
   <si>
     <t>Status of the Device availability.</t>

</xml_diff>